<commit_message>
little changes in raw_date concerning self-report variable
</commit_message>
<xml_diff>
--- a/data/tpack_review_new_16092022.xlsx
+++ b/data/tpack_review_new_16092022.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" codeName="DieseArbeitsmappe"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unitc-my.sharepoint.com/personal/m12aq01_cloud_uni-tuebingen_de/Documents/02-Projekte/02-Review/analysis_new/review_tpack/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\armin\OneDrive - UT Cloud\02-Projekte\02-Review\analysis_new\review_tpack\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="13_ncr:1_{4FCC3A40-22E9-431E-B164-C863C85A01FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9CF9AE0A-0655-4C28-8238-FC7C7AB561A3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B2B49E8-F6DA-42BE-995E-8EEA7536399C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="568" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -274,7 +274,11 @@
     <author>tc={26EA022F-AB57-4F6F-A016-D37BB460C95C}</author>
     <author>tc={F4328141-0057-4D98-B90E-B91E1A179BF9}</author>
     <author>tc={8AB1E830-9C5A-4AEB-8979-3528C75C5C08}</author>
+    <author>tc={0E482D77-F078-45C0-B5F2-7A6302896751}</author>
     <author>tc={BBFCAF67-02B5-4597-9C68-0550A41AE90F}</author>
+    <author>tc={16DB1A0E-E599-4A6B-8064-EFD5F41E7EFA}</author>
+    <author>tc={D331BD9D-5171-45A1-A5CD-A7B7A03527E1}</author>
+    <author>tc={EAC45451-A072-4AA0-8E08-87504ACA46CD}</author>
   </authors>
   <commentList>
     <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{06E0A8B9-0A52-419B-9C0A-5F886B313EE1}">
@@ -453,6 +457,14 @@
         </r>
       </text>
     </comment>
+    <comment ref="BG60" authorId="5" shapeId="0" xr:uid="{0E482D77-F078-45C0-B5F2-7A6302896751}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    (TK=Game knowledge)</t>
+      </text>
+    </comment>
     <comment ref="V74" authorId="0" shapeId="0" xr:uid="{68B4C3A7-9883-4D97-9CFC-7041E3EC5274}">
       <text>
         <r>
@@ -477,7 +489,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B81" authorId="5" shapeId="0" xr:uid="{BBFCAF67-02B5-4597-9C68-0550A41AE90F}">
+    <comment ref="B81" authorId="6" shapeId="0" xr:uid="{BBFCAF67-02B5-4597-9C68-0550A41AE90F}">
       <text>
         <t>[Kommentarthread]
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
@@ -509,12 +521,37 @@
         </r>
       </text>
     </comment>
+    <comment ref="BG93" authorId="7" shapeId="0" xr:uid="{16DB1A0E-E599-4A6B-8064-EFD5F41E7EFA}">
+      <text>
+        <t xml:space="preserve">[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    (N=10)
+</t>
+      </text>
+    </comment>
+    <comment ref="BG100" authorId="8" shapeId="0" xr:uid="{D331BD9D-5171-45A1-A5CD-A7B7A03527E1}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    (Knowledge of Computer Technology)</t>
+      </text>
+    </comment>
+    <comment ref="BG139" authorId="9" shapeId="0" xr:uid="{EAC45451-A072-4AA0-8E08-87504ACA46CD}">
+      <text>
+        <t>[Kommentarthread]
+Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
+Kommentar:
+    SelfEfficacy Scale in Relation to Computer-Based Education (20 items), Computer-assisted Mathematics Instruction Questionnaire (30 items)</t>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4148" uniqueCount="1168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4144" uniqueCount="1168">
   <si>
     <t>authors</t>
   </si>
@@ -4536,6 +4573,7 @@
 
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Armin Fabian" id="{037B00D2-E7C5-419D-A878-F75FC612FA0F}" userId="Armin Fabian" providerId="None"/>
   <person displayName="Kenneth Tulku Kirchner" id="{8C3E2B04-FF9D-471F-A0E9-E33899514011}" userId="Kenneth Tulku Kirchner" providerId="None"/>
   <person displayName="Iris Backfisch" id="{D2B0DC1F-BF8F-4E4B-8298-69B7753638C7}" userId="S::qxoba01@cloud.uni-tuebingen.de::a3c6c389-4f2f-4908-a2e1-9a017b33ba3e" providerId="AD"/>
   <person displayName="Kenneth Tulku Kirchner" id="{5F34A934-A055-44DE-8C56-227E0AA0057E}" userId="S::zxmdn21@s-cloud.uni-tuebingen.de::9952bf8f-ae3d-429a-89db-a497817521cb" providerId="AD"/>
@@ -4831,8 +4869,21 @@
   <threadedComment ref="A11" dT="2021-10-09T09:53:33.68" personId="{5F34A934-A055-44DE-8C56-227E0AA0057E}" id="{8AB1E830-9C5A-4AEB-8979-3528C75C5C08}">
     <text>Full text not available</text>
   </threadedComment>
+  <threadedComment ref="BG60" dT="2022-09-26T14:24:26.22" personId="{037B00D2-E7C5-419D-A878-F75FC612FA0F}" id="{0E482D77-F078-45C0-B5F2-7A6302896751}">
+    <text>(TK=Game knowledge)</text>
+  </threadedComment>
   <threadedComment ref="B81" dT="2022-03-31T08:26:27.23" personId="{8C3E2B04-FF9D-471F-A0E9-E33899514011}" id="{BBFCAF67-02B5-4597-9C68-0550A41AE90F}">
     <text>fies, welche Rubrik?</text>
+  </threadedComment>
+  <threadedComment ref="BG93" dT="2022-09-26T14:24:39.60" personId="{037B00D2-E7C5-419D-A878-F75FC612FA0F}" id="{16DB1A0E-E599-4A6B-8064-EFD5F41E7EFA}">
+    <text xml:space="preserve">(N=10)
+</text>
+  </threadedComment>
+  <threadedComment ref="BG100" dT="2022-09-26T14:24:52.49" personId="{037B00D2-E7C5-419D-A878-F75FC612FA0F}" id="{D331BD9D-5171-45A1-A5CD-A7B7A03527E1}">
+    <text>(Knowledge of Computer Technology)</text>
+  </threadedComment>
+  <threadedComment ref="BG139" dT="2022-09-26T14:25:12.29" personId="{037B00D2-E7C5-419D-A878-F75FC612FA0F}" id="{EAC45451-A072-4AA0-8E08-87504ACA46CD}">
+    <text>SelfEfficacy Scale in Relation to Computer-Based Education (20 items), Computer-assisted Mathematics Instruction Questionnaire (30 items)</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -31900,10 +31951,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F3D981D-54A3-484F-8A98-529030E8793C}">
   <dimension ref="A1:BW140"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="AR1" zoomScale="108" zoomScaleNormal="115" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A131" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="AA1" sqref="AA1"/>
-      <selection pane="bottomLeft" activeCell="H9" sqref="H9"/>
+      <selection pane="bottomLeft" activeCell="BF142" sqref="BF142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7265625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -45222,8 +45273,8 @@
         <f t="shared" si="18"/>
         <v>Asia</v>
       </c>
-      <c r="BG60" s="51" t="s">
-        <v>879</v>
+      <c r="BG60" s="51">
+        <v>1</v>
       </c>
       <c r="BH60" s="51">
         <v>0</v>
@@ -45270,7 +45321,7 @@
       </c>
       <c r="BV60" s="58" t="str">
         <f t="shared" si="17"/>
-        <v>Other</v>
+        <v>TPCK self report, Other</v>
       </c>
     </row>
     <row r="61" spans="1:74" x14ac:dyDescent="0.35">
@@ -52577,8 +52628,8 @@
         <f t="shared" si="27"/>
         <v>Oceania</v>
       </c>
-      <c r="BG93" s="51" t="s">
-        <v>581</v>
+      <c r="BG93" s="51">
+        <v>1</v>
       </c>
       <c r="BH93" s="51">
         <v>24</v>
@@ -52624,9 +52675,9 @@
         <f>0</f>
         <v>0</v>
       </c>
-      <c r="BV93" s="58" t="str">
+      <c r="BV93" s="58" t="e">
         <f t="shared" si="25"/>
-        <v xml:space="preserve">open-ended questionnaire; performance test; interviews; observation; </v>
+        <v>#VALUE!</v>
       </c>
     </row>
     <row r="94" spans="1:74" x14ac:dyDescent="0.35">
@@ -54142,8 +54193,8 @@
         <f t="shared" si="27"/>
         <v>North-America</v>
       </c>
-      <c r="BG100" s="51" t="s">
-        <v>623</v>
+      <c r="BG100" s="51">
+        <v>1</v>
       </c>
       <c r="BH100" s="51">
         <v>25</v>
@@ -54190,7 +54241,7 @@
       </c>
       <c r="BV100" s="58" t="str">
         <f t="shared" si="34"/>
-        <v>Other</v>
+        <v>TPCK self report, 25 Items (); Other</v>
       </c>
     </row>
     <row r="101" spans="1:74" x14ac:dyDescent="0.35">
@@ -60653,7 +60704,7 @@
         <v>0</v>
       </c>
       <c r="F130" s="52" t="str">
-        <f t="shared" ref="F130:F161" si="37">(IF(C130=1,"ICT",)&amp;""&amp;(IF(D130=1,"Educational",))&amp;""&amp;(IF(E130=1,"Subject",)))</f>
+        <f t="shared" ref="F130:F140" si="37">(IF(C130=1,"ICT",)&amp;""&amp;(IF(D130=1,"Educational",))&amp;""&amp;(IF(E130=1,"Subject",)))</f>
         <v>Educational</v>
       </c>
       <c r="G130" s="51" t="s">
@@ -60693,7 +60744,7 @@
         <v>1</v>
       </c>
       <c r="S130" s="52" t="str">
-        <f t="shared" ref="S130:S161" si="38">(IF(L130=1,"TK, ",)&amp;""&amp;(IF(M130=1,"PK, ",))&amp;""&amp;(IF(N130=1,"CK, ",))&amp;""&amp;(IF(O130=1,"TPK, ",))&amp;""&amp;(IF(P130=1,"TCK, ",))&amp;""&amp;(IF(Q130=1,"PCK, ",))&amp;""&amp;(IF(R130=1,"TPCK",)))</f>
+        <f t="shared" ref="S130:S140" si="38">(IF(L130=1,"TK, ",)&amp;""&amp;(IF(M130=1,"PK, ",))&amp;""&amp;(IF(N130=1,"CK, ",))&amp;""&amp;(IF(O130=1,"TPK, ",))&amp;""&amp;(IF(P130=1,"TCK, ",))&amp;""&amp;(IF(Q130=1,"PCK, ",))&amp;""&amp;(IF(R130=1,"TPCK",)))</f>
         <v>TK, TPK, TCK, TPCK</v>
       </c>
       <c r="T130" s="51">
@@ -60749,7 +60800,7 @@
         <v>0</v>
       </c>
       <c r="AK130" s="42">
-        <f t="shared" ref="AK130:AK161" si="40">COUNTIF(AC130:AJ130,"1")</f>
+        <f t="shared" ref="AK130:AK140" si="40">COUNTIF(AC130:AJ130,"1")</f>
         <v>1</v>
       </c>
       <c r="AL130" s="51" t="s">
@@ -60771,7 +60822,7 @@
         <v>0</v>
       </c>
       <c r="AR130" s="51" t="str">
-        <f t="shared" ref="AR130:AR161" si="41">(IF(AN130=1,"quantitative",))&amp;""&amp;(IF(AO130=1,"qualitative",))&amp;""&amp;(IF(AP130=1,"mixed",)&amp;""&amp;(IF(AQ130=1,"non-empirical",)))</f>
+        <f t="shared" ref="AR130:AR140" si="41">(IF(AN130=1,"quantitative",))&amp;""&amp;(IF(AO130=1,"qualitative",))&amp;""&amp;(IF(AP130=1,"mixed",)&amp;""&amp;(IF(AQ130=1,"non-empirical",)))</f>
         <v>quantitative</v>
       </c>
       <c r="AS130" s="51" t="s">
@@ -60787,7 +60838,7 @@
         <v>0</v>
       </c>
       <c r="AW130" s="51" t="str">
-        <f t="shared" ref="AW130:AW161" si="42">(IF(AT130=1,"Pre-service",))&amp;""&amp;(IF(AU130=1,"In-service",))&amp;""&amp;(IF(AV130=1,"Teacher Educator",))</f>
+        <f t="shared" ref="AW130:AW140" si="42">(IF(AT130=1,"Pre-service",))&amp;""&amp;(IF(AU130=1,"In-service",))&amp;""&amp;(IF(AV130=1,"Teacher Educator",))</f>
         <v>Pre-service</v>
       </c>
       <c r="AX130" s="51">
@@ -60856,7 +60907,7 @@
         <v>0</v>
       </c>
       <c r="BV130" s="58" t="e">
-        <f t="shared" ref="BV130:BV161" si="44">IF(BG130=1,"TPCK self report, "&amp;IF(BH130&lt;&gt;0,VALUE(BH130)&amp;" Items ("&amp;IF(BI130&lt;&gt;0,"PK "&amp;VALUE(BI130),)&amp;""&amp;IF(BJ130&lt;&gt;0,", CK "&amp;VALUE(BJ130),)&amp;""&amp;IF(BK130&lt;&gt;0,", TK "&amp;VALUE(BK130),)&amp;""&amp;IF(BL130&lt;&gt;0,", PCK "&amp;VALUE(BL130),)&amp;""&amp;IF(BM130&lt;&gt;0,", TCK "&amp;VALUE(BM130),)&amp;""&amp;IF(BN130&lt;&gt;0,", TPK "&amp;VALUE(BN130),)&amp;""&amp;IF(BO130&lt;&gt;0,", TPCK "&amp;VALUE(BO130),)&amp;"); ",),)&amp;""&amp;IF(BP130=1,"open-ended questionnaire; ",)&amp;""&amp;IF(BQ130=1,"performance test; ",)&amp;""&amp;IF(BR130=1,"interviews; ",)&amp;""&amp;IF(BS130=1,"observation; ",)&amp;""&amp;IF(BU130&lt;&gt;0,"Other",)</f>
+        <f t="shared" ref="BV130:BV140" si="44">IF(BG130=1,"TPCK self report, "&amp;IF(BH130&lt;&gt;0,VALUE(BH130)&amp;" Items ("&amp;IF(BI130&lt;&gt;0,"PK "&amp;VALUE(BI130),)&amp;""&amp;IF(BJ130&lt;&gt;0,", CK "&amp;VALUE(BJ130),)&amp;""&amp;IF(BK130&lt;&gt;0,", TK "&amp;VALUE(BK130),)&amp;""&amp;IF(BL130&lt;&gt;0,", PCK "&amp;VALUE(BL130),)&amp;""&amp;IF(BM130&lt;&gt;0,", TCK "&amp;VALUE(BM130),)&amp;""&amp;IF(BN130&lt;&gt;0,", TPK "&amp;VALUE(BN130),)&amp;""&amp;IF(BO130&lt;&gt;0,", TPCK "&amp;VALUE(BO130),)&amp;"); ",),)&amp;""&amp;IF(BP130=1,"open-ended questionnaire; ",)&amp;""&amp;IF(BQ130=1,"performance test; ",)&amp;""&amp;IF(BR130=1,"interviews; ",)&amp;""&amp;IF(BS130=1,"observation; ",)&amp;""&amp;IF(BU130&lt;&gt;0,"Other",)</f>
         <v>#VALUE!</v>
       </c>
     </row>
@@ -62813,8 +62864,8 @@
       <c r="BF139" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="BG139" s="51" t="s">
-        <v>455</v>
+      <c r="BG139" s="51">
+        <v>1</v>
       </c>
       <c r="BH139" s="51">
         <v>0</v>
@@ -62861,7 +62912,7 @@
       </c>
       <c r="BV139" s="58" t="str">
         <f t="shared" si="44"/>
-        <v>interviews; observation; Other</v>
+        <v>TPCK self report, interviews; observation; Other</v>
       </c>
     </row>
     <row r="140" spans="1:74" x14ac:dyDescent="0.35">
@@ -63111,18 +63162,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -63355,18 +63406,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDCBDF50-ED16-43B9-8B09-0A4A16ED3483}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EAF23D1-FB8B-4F69-BC9E-B6E5E2241335}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5EAF23D1-FB8B-4F69-BC9E-B6E5E2241335}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDCBDF50-ED16-43B9-8B09-0A4A16ED3483}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>